<commit_message>
updated demo content assessment outputs
</commit_message>
<xml_diff>
--- a/demo_files/output/Complexity.xlsx
+++ b/demo_files/output/Complexity.xlsx
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\avg_sal.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\avg_sal.sql</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -542,7 +542,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\cursor.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\cursor.sql</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\error_handle.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\error_handle.sql</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -626,7 +626,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\loop.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\loop.sql</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\nestloop.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\nestloop.sql</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\stringfunc.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\stringfunc.sql</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -752,7 +752,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\billing.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\billing.sql</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -794,7 +794,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\employee_ops.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\employee_ops.sql</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -836,7 +836,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\error_handling.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\error_handling.sql</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\financial_ops.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\financial_ops.sql</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -920,7 +920,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\general_ops.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\general_ops.sql</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -962,7 +962,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\inventory_ops.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\inventory_ops.sql</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1004,7 +1004,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\payroll_ops.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\payroll_ops.sql</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1046,7 +1046,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\product_ops.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\product_ops.sql</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\PLSQL\JTA\triggers.sql</t>
+          <t>demo_files/DEMO_DB\PLSQL\JTA\triggers.sql</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1236,7 +1236,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\SQR\data_inserter.sqr</t>
+          <t>demo_files/DEMO_DB\SQR\data_inserter.sqr</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1293,7 +1293,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\SQR\dates.sqr</t>
+          <t>demo_files/DEMO_DB\SQR\dates.sqr</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1350,7 +1350,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\SQR\excel.sqr</t>
+          <t>demo_files/DEMO_DB\SQR\excel.sqr</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1407,7 +1407,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\SQR\multiple_rep.sqr</t>
+          <t>demo_files/DEMO_DB\SQR\multiple_rep.sqr</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1464,7 +1464,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\SQR\process_name.sqr</t>
+          <t>demo_files/DEMO_DB\SQR\process_name.sqr</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report.et</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1652,7 +1652,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report10.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report10.et</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1697,7 +1697,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report2.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report2.et</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1742,7 +1742,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report3.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report3.et</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1787,7 +1787,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report4.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report4.et</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1832,7 +1832,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report5.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report5.et</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1877,7 +1877,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report6.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report6.et</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1922,7 +1922,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report7.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report7.et</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1967,7 +1967,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report8.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report8.et</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2012,7 +2012,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>files/content_assessment/DEMO_DB\EasyTrieve\report9.et</t>
+          <t>demo_files/DEMO_DB\EasyTrieve\report9.et</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">

</xml_diff>